<commit_message>
Implemented State Filtering in HUD Tab
- HUD averages now can be filtered by state like FMR & PHA
- Fixed test data in HUD Test Excel
</commit_message>
<xml_diff>
--- a/Test Excels/HUD_Crawler_Test_Excel.xlsx
+++ b/Test Excels/HUD_Crawler_Test_Excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\SectionM8 Business Documents\SectionM8 Fall 2025 Demo\SectionM8-Demo-Fall2025\Test Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1A7AE2-FA43-4B1D-B39D-97252E655721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AF5898-484C-416C-9F2C-6512E498D379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -866,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1099,7 +1099,7 @@
         <v>19406</v>
       </c>
       <c r="L2">
-        <v>101000</v>
+        <v>85000</v>
       </c>
       <c r="M2">
         <v>24000</v>
@@ -1129,7 +1129,7 @@
         <v>50</v>
       </c>
       <c r="V2">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="W2">
         <v>6.5000000000000002E-2</v>
@@ -1281,7 +1281,7 @@
         <v>19320</v>
       </c>
       <c r="L3">
-        <v>95000</v>
+        <v>85000</v>
       </c>
       <c r="M3">
         <v>30000</v>
@@ -1311,7 +1311,7 @@
         <v>134</v>
       </c>
       <c r="V3">
-        <v>131</v>
+        <v>100</v>
       </c>
       <c r="W3">
         <v>2.1999999999999999E-2</v>
@@ -1493,7 +1493,7 @@
         <v>89</v>
       </c>
       <c r="V4">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="W4">
         <v>0.10100000000000001</v>
@@ -1675,7 +1675,7 @@
         <v>133</v>
       </c>
       <c r="V5">
-        <v>130</v>
+        <v>67</v>
       </c>
       <c r="W5">
         <v>2.3E-2</v>
@@ -1857,7 +1857,7 @@
         <v>102</v>
       </c>
       <c r="V6">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="W6">
         <v>2.9000000000000001E-2</v>
@@ -2039,7 +2039,7 @@
         <v>48</v>
       </c>
       <c r="V7">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="W7">
         <v>6.2E-2</v>
@@ -2221,7 +2221,7 @@
         <v>125</v>
       </c>
       <c r="V8">
-        <v>124</v>
+        <v>76</v>
       </c>
       <c r="W8">
         <v>8.0000000000000002E-3</v>

</xml_diff>